<commit_message>
version0.3: added multiple window sizes, fixed bugs
the user can change the processing window sizes (epochs) and the tool recalculates data.
</commit_message>
<xml_diff>
--- a/MainReport.xlsx
+++ b/MainReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>P002 90 Degrees per second T1 Left.csv</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>MDF</t>
+  </si>
+  <si>
+    <t>grid1</t>
+  </si>
+  <si>
+    <t>grid2</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>RMS</t>
   </si>
   <si>
     <t>grid1</t>
@@ -118,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -128,14 +140,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -758,6 +774,62 @@
         <v>4.4253600949560843</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="0">
+        <v>4.9837033567055027</v>
+      </c>
+      <c r="E6" s="0">
+        <v>7.6154278127341932</v>
+      </c>
+      <c r="F6" s="0">
+        <v>-0.42355894430186491</v>
+      </c>
+      <c r="G6" s="0">
+        <v>-0.39515686533869077</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.37708656173945287</v>
+      </c>
+      <c r="I6" s="0">
+        <v>2.444139291155317</v>
+      </c>
+      <c r="J6" s="0">
+        <v>4.4169010412501262</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="0">
+        <v>4.8132933006222851</v>
+      </c>
+      <c r="M6" s="0">
+        <v>26.497697273869736</v>
+      </c>
+      <c r="N6" s="0">
+        <v>-0.25380222280809078</v>
+      </c>
+      <c r="O6" s="0">
+        <v>-0.40754931110034676</v>
+      </c>
+      <c r="P6" s="0">
+        <v>0.55743954844668608</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>2.6769939795094224</v>
+      </c>
+      <c r="R6" s="0">
+        <v>4.8598205241911741</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 0.4, fixed bugs and improve optimization
* added load_defaults, allows user to restart without closing the HDEMG_Settings
* fixed nansum error
* fixed filtering, added sampling frequency
* fixed MDF calculation, added sampling frequency
* fixed ARV calculation
* fixed no Aux plot
* added epoch_ms to the reports
</commit_message>
<xml_diff>
--- a/MainReport.xlsx
+++ b/MainReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprad\Documents\MATLAB\Project_UK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62BA934-9B1A-4756-9B8A-D20A28C8D7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5662CC-ECA8-46D0-95BC-433D186A60F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>P002 90 Degrees per second T1 Left.csv</t>
   </si>
@@ -92,6 +92,45 @@
   </si>
   <si>
     <t>MDF</t>
+  </si>
+  <si>
+    <t>grid1</t>
+  </si>
+  <si>
+    <t>grid2</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>grid1</t>
+  </si>
+  <si>
+    <t>grid2</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>grid1</t>
+  </si>
+  <si>
+    <t>grid2</t>
+  </si>
+  <si>
+    <t>Epoch_ms</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>RMS</t>
   </si>
   <si>
     <t>grid1</t>
@@ -130,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,19 +178,13 @@
       <diagonal/>
     </border>
     <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,32 +499,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="33.15625" customWidth="true"/>
     <col min="2" max="2" width="7.37890625" customWidth="true"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true"/>
-    <col min="8" max="8" width="13.7109375" customWidth="true"/>
-    <col min="9" max="9" width="11.7109375" customWidth="true"/>
-    <col min="12" max="12" width="11.7109375" customWidth="true"/>
-    <col min="14" max="14" width="13.37890625" customWidth="true"/>
-    <col min="16" max="16" width="14.7109375" customWidth="true"/>
-    <col min="17" max="17" width="11.7109375" customWidth="true"/>
-    <col min="3" max="3" width="5.15625" customWidth="true"/>
+    <col min="3" max="3" width="9.48828125" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="5.15625" customWidth="true"/>
     <col min="5" max="5" width="11.7109375" customWidth="true"/>
-    <col min="6" max="6" width="13.37890625" customWidth="true"/>
-    <col min="7" max="7" width="17.7109375" customWidth="true"/>
+    <col min="7" max="7" width="14.37890625" customWidth="true"/>
+    <col min="8" max="8" width="17.7109375" customWidth="true"/>
+    <col min="9" max="9" width="13.7109375" customWidth="true"/>
     <col min="10" max="10" width="11.7109375" customWidth="true"/>
-    <col min="11" max="11" width="5.15625" customWidth="true"/>
+    <col min="12" max="12" width="5.15625" customWidth="true"/>
     <col min="13" max="13" width="11.7109375" customWidth="true"/>
-    <col min="15" max="15" width="17.7109375" customWidth="true"/>
+    <col min="15" max="15" width="13.37890625" customWidth="true"/>
+    <col min="16" max="16" width="17.7109375" customWidth="true"/>
+    <col min="17" max="17" width="14.7109375" customWidth="true"/>
     <col min="18" max="18" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="11.7109375" customWidth="true"/>
+    <col min="19" max="19" width="11.7109375" customWidth="true"/>
+    <col min="20" max="20" width="11.6640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -502,51 +537,54 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -557,52 +595,52 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4.8890408834650172</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>20.688569590855167</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>-0.30250130218943166</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-0.22017104177711372</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.49830896183771489</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2.6588583266832657</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>4.5112100912991719</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>4.9735989513174905</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>9.7553337715042172</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>-0.21279910108677727</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>-0.2270273451197832</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.61263372248664871</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>2.4452917297097208</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>4.4977165813022584</v>
       </c>
     </row>
@@ -613,221 +651,398 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4.8890408834650172</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>20.688569590855167</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>-0.30250130218943166</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-0.22017104177711372</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.49830896183771489</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2.6588583266832657</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>4.5112100912991719</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>4.9735989513174905</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>9.7553337715042172</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>-0.21279910108677727</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>-0.2270273451197832</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.61263372248664871</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2.4452917297097208</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>4.4977165813022584</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0">
+      <c r="E4">
         <v>4.7918728474103682</v>
       </c>
-      <c r="E4" s="0">
+      <c r="F4">
         <v>28.416757608795852</v>
       </c>
-      <c r="F4" s="0">
+      <c r="G4">
         <v>-1.8869422788754013</v>
       </c>
-      <c r="G4" s="0">
+      <c r="H4">
         <v>-1.7899628898574858</v>
       </c>
-      <c r="H4" s="0">
-        <v>0.012973516876859411</v>
-      </c>
-      <c r="I4" s="0">
+      <c r="I4">
+        <v>1.2973516876859411E-2</v>
+      </c>
+      <c r="J4">
         <v>2.3129561572495949</v>
       </c>
-      <c r="J4" s="0">
+      <c r="K4">
         <v>4.6048921158152876</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="0">
+      <c r="M4">
         <v>4.560284284529958</v>
       </c>
-      <c r="M4" s="0">
+      <c r="N4">
         <v>46.727015605099496</v>
       </c>
-      <c r="N4" s="0">
+      <c r="O4">
         <v>-2.0863476699963575</v>
       </c>
-      <c r="O4" s="0">
+      <c r="P4">
         <v>-1.8936522825686257</v>
       </c>
-      <c r="P4" s="0">
-        <v>0.0081969508310558593</v>
-      </c>
-      <c r="Q4" s="0">
+      <c r="Q4">
+        <v>8.1969508310558593E-3</v>
+      </c>
+      <c r="R4">
         <v>2.4514775672635611</v>
       </c>
-      <c r="R4" s="0">
+      <c r="S4">
         <v>4.415173640918117</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="0">
+      <c r="E5">
         <v>4.9989472758971347</v>
       </c>
-      <c r="E5" s="0">
+      <c r="F5">
         <v>1.9449199480593771</v>
       </c>
-      <c r="F5" s="0">
+      <c r="G5">
         <v>1.7104840201196674</v>
       </c>
-      <c r="G5" s="0">
+      <c r="H5">
         <v>1.7114195983342617</v>
       </c>
-      <c r="H5" s="0">
+      <c r="I5">
         <v>51.343328536008464</v>
       </c>
-      <c r="I5" s="0">
+      <c r="J5">
         <v>2.5025997126108903</v>
       </c>
-      <c r="J5" s="0">
+      <c r="K5">
         <v>4.5358690089822566</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="0">
+      <c r="M5">
         <v>4.9944534538591236</v>
       </c>
-      <c r="M5" s="0">
+      <c r="N5">
         <v>4.4796174098101176</v>
       </c>
-      <c r="N5" s="0">
+      <c r="O5">
         <v>1.7141421451587313</v>
       </c>
-      <c r="O5" s="0">
+      <c r="P5">
         <v>1.7272100324941175</v>
       </c>
-      <c r="P5" s="0">
+      <c r="Q5">
         <v>51.777627307937649</v>
       </c>
-      <c r="Q5" s="0">
+      <c r="R5">
         <v>2.5087379302233117</v>
       </c>
-      <c r="R5" s="0">
+      <c r="S5">
         <v>4.4253600949560843</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="0">
+      <c r="E6">
         <v>4.9837033567055027</v>
       </c>
-      <c r="E6" s="0">
+      <c r="F6">
         <v>7.6154278127341932</v>
       </c>
-      <c r="F6" s="0">
+      <c r="G6">
         <v>-0.42355894430186491</v>
       </c>
-      <c r="G6" s="0">
+      <c r="H6">
         <v>-0.39515686533869077</v>
       </c>
-      <c r="H6" s="0">
+      <c r="I6">
         <v>0.37708656173945287</v>
       </c>
-      <c r="I6" s="0">
+      <c r="J6">
         <v>2.444139291155317</v>
       </c>
-      <c r="J6" s="0">
+      <c r="K6">
         <v>4.4169010412501262</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="0">
+      <c r="M6">
         <v>4.8132933006222851</v>
       </c>
-      <c r="M6" s="0">
+      <c r="N6">
         <v>26.497697273869736</v>
       </c>
-      <c r="N6" s="0">
+      <c r="O6">
         <v>-0.25380222280809078</v>
       </c>
-      <c r="O6" s="0">
+      <c r="P6">
         <v>-0.40754931110034676</v>
       </c>
-      <c r="P6" s="0">
+      <c r="Q6">
         <v>0.55743954844668608</v>
       </c>
-      <c r="Q6" s="0">
+      <c r="R6">
         <v>2.6769939795094224</v>
       </c>
-      <c r="R6" s="0">
+      <c r="S6">
         <v>4.8598205241911741</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>4.9588780618938761</v>
+      </c>
+      <c r="F7">
+        <v>12.545291530466567</v>
+      </c>
+      <c r="G7">
+        <v>1.5807298502341013E-2</v>
+      </c>
+      <c r="H7">
+        <v>5.8012369885457465E-2</v>
+      </c>
+      <c r="I7">
+        <v>1.0370681545480136</v>
+      </c>
+      <c r="J7">
+        <v>2.475928634483771</v>
+      </c>
+      <c r="K7">
+        <v>4.6440778216633722</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7">
+        <v>4.9887881872439932</v>
+      </c>
+      <c r="N7">
+        <v>6.3685566438740695</v>
+      </c>
+      <c r="O7">
+        <v>-0.29230080263954372</v>
+      </c>
+      <c r="P7">
+        <v>-0.29205796332092832</v>
+      </c>
+      <c r="Q7">
+        <v>0.51015153455024853</v>
+      </c>
+      <c r="R7">
+        <v>2.4917443630776885</v>
+      </c>
+      <c r="S7">
+        <v>4.5274373986541478</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <v>4.9565796033598728</v>
+      </c>
+      <c r="F8">
+        <v>12.898599613166178</v>
+      </c>
+      <c r="G8">
+        <v>-1.9577033441519488E-2</v>
+      </c>
+      <c r="H8">
+        <v>5.7393201234815262E-3</v>
+      </c>
+      <c r="I8">
+        <v>0.95592312210974395</v>
+      </c>
+      <c r="J8">
+        <v>2.4859649460484721</v>
+      </c>
+      <c r="K8">
+        <v>4.679845026918132</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8">
+        <v>4.9589499261234549</v>
+      </c>
+      <c r="N8">
+        <v>12.066529840571235</v>
+      </c>
+      <c r="O8">
+        <v>-0.30732425914533296</v>
+      </c>
+      <c r="P8">
+        <v>-0.34674311669755931</v>
+      </c>
+      <c r="Q8">
+        <v>0.49280572091851571</v>
+      </c>
+      <c r="R8">
+        <v>2.5327498430948712</v>
+      </c>
+      <c r="S8">
+        <v>4.6844664277032386</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="0">
+        <v>250</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="0">
+        <v>4.9840659413546451</v>
+      </c>
+      <c r="F9" s="0">
+        <v>7.5834772869910072</v>
+      </c>
+      <c r="G9" s="0">
+        <v>-0.80979371002369249</v>
+      </c>
+      <c r="H9" s="0">
+        <v>-0.78373119768272148</v>
+      </c>
+      <c r="I9" s="0">
+        <v>0.15495524819075412</v>
+      </c>
+      <c r="J9" s="0">
+        <v>2.4829695786248123</v>
+      </c>
+      <c r="K9" s="0">
+        <v>4.3331189827446321</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="0">
+        <v>4.87773921722256</v>
+      </c>
+      <c r="N9" s="0">
+        <v>21.136591178998778</v>
+      </c>
+      <c r="O9" s="0">
+        <v>-0.6377922115169995</v>
+      </c>
+      <c r="P9" s="0">
+        <v>-0.72352412303316482</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>0.23025432072322813</v>
+      </c>
+      <c r="R9" s="0">
+        <v>2.6872302464371898</v>
+      </c>
+      <c r="S9" s="0">
+        <v>4.7166052310639204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a metric: contraction index, fixed bugs
* added co-contraction index
* added manual entry for grid layout
</commit_message>
<xml_diff>
--- a/MainReport.xlsx
+++ b/MainReport.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprad\Documents\MATLAB\Project_UK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF347ED3-C25B-4170-B359-8AD8DC71B5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21637FA1-CA67-4618-8B42-8BDCF037EB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Filename</t>
   </si>
@@ -55,16 +55,22 @@
     <t>Epoch_ms</t>
   </si>
   <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>CCI</t>
+  </si>
+  <si>
     <t>L120.csv</t>
   </si>
   <si>
     <t>RMS</t>
   </si>
   <si>
-    <t>grid1</t>
-  </si>
-  <si>
-    <t>grid2</t>
+    <t>grid1:32</t>
+  </si>
+  <si>
+    <t>grid2:32</t>
   </si>
   <si>
     <t>L120.csv</t>
@@ -73,25 +79,34 @@
     <t>RMS</t>
   </si>
   <si>
-    <t>grid1</t>
-  </si>
-  <si>
-    <t>grid2</t>
-  </si>
-  <si>
-    <t>Max</t>
+    <t>grid1:32</t>
+  </si>
+  <si>
+    <t>grid2:32</t>
   </si>
   <si>
     <t>L120.csv</t>
   </si>
   <si>
+    <t>MDF</t>
+  </si>
+  <si>
+    <t>grid1:32</t>
+  </si>
+  <si>
+    <t>grid2:32</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
     <t>RMS</t>
   </si>
   <si>
-    <t>grid1</t>
-  </si>
-  <si>
-    <t>grid2</t>
+    <t>grid1:28</t>
+  </si>
+  <si>
+    <t>grid2:28</t>
   </si>
   <si>
     <t>L120.csv</t>
@@ -100,22 +115,34 @@
     <t>RMS</t>
   </si>
   <si>
-    <t>grid1</t>
-  </si>
-  <si>
-    <t>grid2</t>
+    <t>grid1:28</t>
+  </si>
+  <si>
+    <t>grid2:28</t>
   </si>
   <si>
     <t>L120.csv</t>
   </si>
   <si>
-    <t>RMS</t>
-  </si>
-  <si>
-    <t>grid1</t>
-  </si>
-  <si>
-    <t>grid2</t>
+    <t>MDF</t>
+  </si>
+  <si>
+    <t>grid1:28</t>
+  </si>
+  <si>
+    <t>grid2:28</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>MDF</t>
+  </si>
+  <si>
+    <t>grid1:28</t>
+  </si>
+  <si>
+    <t>grid2:28</t>
   </si>
 </sst>
 </file>
@@ -136,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -144,12 +171,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,34 +493,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.109375" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" customWidth="1"/>
-    <col min="11" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" customWidth="1"/>
-    <col min="14" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" customWidth="1"/>
-    <col min="19" max="19" width="4.6640625" customWidth="1"/>
-    <col min="20" max="22" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.48828125" customWidth="true"/>
+    <col min="2" max="2" width="7.37890625" customWidth="true"/>
+    <col min="3" max="3" width="9.48828125" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="7.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="13.37890625" customWidth="true"/>
+    <col min="8" max="8" width="17.7109375" customWidth="true"/>
+    <col min="9" max="9" width="13.7109375" customWidth="true"/>
+    <col min="10" max="10" width="6.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="13" max="13" width="7.7109375" customWidth="true"/>
+    <col min="14" max="14" width="11.7109375" customWidth="true"/>
+    <col min="16" max="16" width="13.7109375" customWidth="true"/>
+    <col min="17" max="17" width="17.7109375" customWidth="true"/>
+    <col min="18" max="18" width="12.7109375" customWidth="true"/>
+    <col min="19" max="19" width="6.7109375" customWidth="true"/>
+    <col min="20" max="20" width="11.7109375" customWidth="true"/>
+    <col min="22" max="22" width="12.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="12" max="12" width="11.7109375" customWidth="true"/>
+    <col min="15" max="15" width="11.7109375" customWidth="true"/>
+    <col min="21" max="21" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -547,7 +581,7 @@
         <v>6</v>
       </c>
       <c r="S1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="T1" t="s">
         <v>7</v>
@@ -555,324 +589,484 @@
       <c r="U1" t="s">
         <v>8</v>
       </c>
+      <c r="V1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>4.9491413643144613</v>
+        <v>4.9826449068195009</v>
       </c>
       <c r="F2">
-        <v>13.504878241869031</v>
+        <v>7.9001322104036635</v>
       </c>
       <c r="G2">
-        <v>-7.3346433597391486E-2</v>
+        <v>-0.22685820616857416</v>
       </c>
       <c r="H2">
-        <v>-5.1484168601886818E-3</v>
+        <v>-0.2073975249232469</v>
       </c>
       <c r="I2">
-        <v>0.84460484114001155</v>
+        <v>0.59311894177556757</v>
+      </c>
+      <c r="J2">
+        <v>1.65</v>
       </c>
       <c r="K2">
-        <v>2.3892410675555888</v>
+        <v>2.5037162017088295</v>
       </c>
       <c r="L2">
-        <v>4.4733271645787847</v>
+        <v>4.3232609635970078</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N2">
-        <v>4.8790566878423807</v>
+        <v>4.7356539370070294</v>
       </c>
       <c r="O2">
-        <v>21.031988398531791</v>
+        <v>31.65087027615273</v>
       </c>
       <c r="P2">
-        <v>-0.11448682523315389</v>
+        <v>5.7096888284919711E-2</v>
       </c>
       <c r="Q2">
-        <v>-0.21059076169776025</v>
+        <v>-9.3042982720196218E-2</v>
       </c>
       <c r="R2">
-        <v>0.76826876154361645</v>
+        <v>1.1405041982782089</v>
+      </c>
+      <c r="S2">
+        <v>2.25</v>
       </c>
       <c r="T2">
-        <v>2.6415567347611328</v>
+        <v>2.7323295115112365</v>
       </c>
       <c r="U2">
-        <v>4.8049314794734164</v>
+        <v>4.9555216526329442</v>
+      </c>
+      <c r="V2">
+        <v>0.5745467581032272</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>250</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3">
-        <v>4.9625569479790368</v>
+        <v>4.9827541319052324</v>
       </c>
       <c r="F3">
-        <v>11.894689205470186</v>
+        <v>7.8740373620503528</v>
       </c>
       <c r="G3">
-        <v>5.8665361850126642E-2</v>
+        <v>-0.22747177973472568</v>
       </c>
       <c r="H3">
-        <v>0.10417119977348441</v>
+        <v>-0.20824049978381717</v>
       </c>
       <c r="I3">
-        <v>1.1446306261037507</v>
+        <v>0.59228157182295083</v>
       </c>
       <c r="J3">
-        <v>0.68</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>2.4468107223221605</v>
+        <v>2.5041788721098985</v>
       </c>
       <c r="L3">
-        <v>4.60079565205411</v>
+        <v>4.3239160808207764</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N3">
-        <v>4.9942425642727555</v>
+        <v>4.7404864785606913</v>
       </c>
       <c r="O3">
-        <v>4.6303042176411786</v>
+        <v>31.350721975264484</v>
       </c>
       <c r="P3">
-        <v>-0.23007455991915735</v>
+        <v>5.6693418498374525E-2</v>
       </c>
       <c r="Q3">
-        <v>-0.21861465470759606</v>
+        <v>-9.1493144296735884E-2</v>
       </c>
       <c r="R3">
-        <v>0.58874257102539052</v>
+        <v>1.1394451350814223</v>
       </c>
       <c r="S3">
-        <v>0.31</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>2.4927126270953548</v>
+        <v>2.729627503259529</v>
       </c>
       <c r="U3">
-        <v>4.4952212915808447</v>
+        <v>4.9528656752405942</v>
+      </c>
+      <c r="V3">
+        <v>0.57341559073516013</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4">
-        <v>4.9831631184508538</v>
+        <v>4.9997147825811075</v>
       </c>
       <c r="F4">
-        <v>7.7711595435337895</v>
+        <v>1.0123546844457523</v>
       </c>
       <c r="G4">
-        <v>-0.25837251282338408</v>
+        <v>2.1850623651544141</v>
       </c>
       <c r="H4">
-        <v>-0.23970770529510779</v>
+        <v>2.1877179967923386</v>
       </c>
       <c r="I4">
-        <v>0.55160410204185617</v>
+        <v>153.13073432744957</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>303.02999999999997</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>2.4913278861865829</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>4.4964457027896536</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N4">
-        <v>4.7228568332940331</v>
+        <v>4.957208825138796</v>
       </c>
       <c r="O4">
-        <v>32.623824683273597</v>
+        <v>12.455041257342652</v>
       </c>
       <c r="P4">
-        <v>4.7973641343654269E-2</v>
+        <v>2.116146697895704</v>
       </c>
       <c r="Q4">
-        <v>-0.11175036265998851</v>
+        <v>2.1757732740706923</v>
       </c>
       <c r="R4">
-        <v>1.1167954640015669</v>
+        <v>130.66121667900043</v>
       </c>
       <c r="S4">
-        <v>2.39</v>
+        <v>222.22</v>
       </c>
       <c r="T4">
-        <v>2.7418393910877636</v>
+        <v>2.4563775322756314</v>
       </c>
       <c r="U4">
-        <v>4.9740466377912309</v>
+        <v>4.2481080206193091</v>
+      </c>
+      <c r="V4">
+        <v>1.1889440487387544</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>4.97984594877299</v>
+        <v>4.6798586414822303</v>
       </c>
       <c r="F5">
-        <v>8.5095082415976222</v>
+        <v>21.311092513734366</v>
       </c>
       <c r="G5">
-        <v>-0.23158218546749429</v>
+        <v>-1.3481989837480159</v>
       </c>
       <c r="H5">
-        <v>-0.2121461353955239</v>
+        <v>-1.389217402286778</v>
       </c>
       <c r="I5">
-        <v>0.58670233213120249</v>
+        <v>4.4853983220576397E-2</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2.5816969466091404</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>3.7150696060018951</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N5">
-        <v>4.7291322092057975</v>
+        <v>4.4875707068022246</v>
       </c>
       <c r="O5">
-        <v>32.359327747518378</v>
+        <v>37.001887552688956</v>
       </c>
       <c r="P5">
-        <v>7.7851326465882678E-2</v>
+        <v>-0.64876785580293639</v>
       </c>
       <c r="Q5">
-        <v>-8.3462151450959615E-2</v>
+        <v>-0.51183675017913821</v>
       </c>
       <c r="R5">
-        <v>1.196330917092719</v>
+        <v>0.22450816705765561</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>0.44</v>
       </c>
       <c r="T5">
-        <v>2.7287266387098681</v>
+        <v>2.7441176564680601</v>
       </c>
       <c r="U5">
-        <v>4.9936107520270854</v>
+        <v>4.0971384291796884</v>
+      </c>
+      <c r="V5">
+        <v>0.23414038748356941</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>4.9831099143356452</v>
+        <v>4.7026976035184864</v>
       </c>
       <c r="F6">
-        <v>7.8028732011856921</v>
+        <v>19.255097091802149</v>
       </c>
       <c r="G6">
-        <v>-0.18003493500524359</v>
+        <v>-1.3362678808654391</v>
       </c>
       <c r="H6">
-        <v>-0.15930437258937813</v>
+        <v>-1.3941377130566481</v>
       </c>
       <c r="I6">
-        <v>0.66064030342087743</v>
+        <v>4.6103311309136655E-2</v>
       </c>
       <c r="J6">
-        <v>1.65</v>
+        <v>0.62</v>
       </c>
       <c r="K6">
-        <v>2.5022422143484819</v>
+        <v>2.6016446203947199</v>
       </c>
       <c r="L6">
-        <v>4.3254144498818148</v>
+        <v>3.8350165554762237</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N6">
-        <v>4.670776579670628</v>
+        <v>4.4612663544296156</v>
       </c>
       <c r="O6">
-        <v>35.318252487446763</v>
+        <v>38.786048126058219</v>
       </c>
       <c r="P6">
-        <v>8.9733138721553293E-2</v>
+        <v>-0.63296529236637555</v>
       </c>
       <c r="Q6">
-        <v>-7.132827650629267E-2</v>
+        <v>-0.5012775858011308</v>
       </c>
       <c r="R6">
-        <v>1.2295130387859479</v>
+        <v>0.23282773198201309</v>
       </c>
       <c r="S6">
-        <v>2.25</v>
+        <v>0.4</v>
       </c>
       <c r="T6">
-        <v>2.7400123957538387</v>
+        <v>2.76557150664777</v>
       </c>
       <c r="U6">
-        <v>5.0263168840937595</v>
+        <v>4.0668101682719353</v>
+      </c>
+      <c r="V6">
+        <v>0.23539846667524203</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>4.7906418405145521</v>
+      </c>
+      <c r="F7">
+        <v>7.8095861425232034</v>
+      </c>
+      <c r="G7">
+        <v>2.0677957682929509</v>
+      </c>
+      <c r="H7">
+        <v>2.0736812204762769</v>
+      </c>
+      <c r="I7">
+        <v>116.89495504965939</v>
+      </c>
+      <c r="J7">
+        <v>500</v>
+      </c>
+      <c r="K7">
+        <v>2.4955351463113833</v>
+      </c>
+      <c r="L7">
+        <v>4.1235868656811236</v>
+      </c>
+      <c r="M7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7">
+        <v>4.7126536062264037</v>
+      </c>
+      <c r="O7">
+        <v>18.377104569427054</v>
+      </c>
+      <c r="P7">
+        <v>2.0355298942327686</v>
+      </c>
+      <c r="Q7">
+        <v>2.0220858840864073</v>
+      </c>
+      <c r="R7">
+        <v>108.52502491934652</v>
+      </c>
+      <c r="S7">
+        <v>500</v>
+      </c>
+      <c r="T7">
+        <v>2.4589208462812953</v>
+      </c>
+      <c r="U7">
+        <v>4.2481821928316998</v>
+      </c>
+      <c r="V7">
+        <v>1.099828617014579</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0">
+        <v>500</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="0">
+        <v>4.7906418405145521</v>
+      </c>
+      <c r="F8" s="0">
+        <v>7.8095861425232034</v>
+      </c>
+      <c r="G8" s="0">
+        <v>2.0677957682929509</v>
+      </c>
+      <c r="H8" s="0">
+        <v>2.0736812204762769</v>
+      </c>
+      <c r="I8" s="0">
+        <v>116.89495504965939</v>
+      </c>
+      <c r="J8" s="0">
+        <v>500</v>
+      </c>
+      <c r="K8" s="0">
+        <v>2.4955351463113833</v>
+      </c>
+      <c r="L8" s="0">
+        <v>4.1235868656811236</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="0">
+        <v>4.7126536062264037</v>
+      </c>
+      <c r="O8" s="0">
+        <v>18.377104569427054</v>
+      </c>
+      <c r="P8" s="0">
+        <v>2.0355298942327686</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2.0220858840864073</v>
+      </c>
+      <c r="R8" s="0">
+        <v>108.52502491934652</v>
+      </c>
+      <c r="S8" s="0">
+        <v>500</v>
+      </c>
+      <c r="T8" s="0">
+        <v>2.4589208462812953</v>
+      </c>
+      <c r="U8" s="0">
+        <v>4.2481821928316998</v>
+      </c>
+      <c r="V8" s="0">
+        <v>1.099828617014579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major Update: added layouts
* added 3 basic configurations: 32, 64, 64_Long
* specific functions for mono to bipolar converter and maping functions
* users can assign grid layouts in such configuration
</commit_message>
<xml_diff>
--- a/MainReport.xlsx
+++ b/MainReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprad\Documents\MATLAB\Project_UK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21637FA1-CA67-4618-8B42-8BDCF037EB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F45AAE-07D6-42A2-BACB-26B28E7CD6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Filename</t>
   </si>
@@ -85,10 +85,13 @@
     <t>grid2:32</t>
   </si>
   <si>
+    <t>Index</t>
+  </si>
+  <si>
     <t>L120.csv</t>
   </si>
   <si>
-    <t>MDF</t>
+    <t>ARV</t>
   </si>
   <si>
     <t>grid1:32</t>
@@ -100,6 +103,18 @@
     <t>L120.csv</t>
   </si>
   <si>
+    <t>ARV</t>
+  </si>
+  <si>
+    <t>grid1:32</t>
+  </si>
+  <si>
+    <t>grid2:32</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
     <t>RMS</t>
   </si>
   <si>
@@ -113,30 +128,6 @@
   </si>
   <si>
     <t>RMS</t>
-  </si>
-  <si>
-    <t>grid1:28</t>
-  </si>
-  <si>
-    <t>grid2:28</t>
-  </si>
-  <si>
-    <t>L120.csv</t>
-  </si>
-  <si>
-    <t>MDF</t>
-  </si>
-  <si>
-    <t>grid1:28</t>
-  </si>
-  <si>
-    <t>grid2:28</t>
-  </si>
-  <si>
-    <t>L120.csv</t>
-  </si>
-  <si>
-    <t>MDF</t>
   </si>
   <si>
     <t>grid1:28</t>
@@ -493,36 +484,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.48828125" customWidth="true"/>
     <col min="2" max="2" width="7.37890625" customWidth="true"/>
-    <col min="3" max="3" width="9.48828125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="7.7109375" customWidth="true"/>
-    <col min="5" max="5" width="11.7109375" customWidth="true"/>
-    <col min="7" max="7" width="13.37890625" customWidth="true"/>
-    <col min="8" max="8" width="17.7109375" customWidth="true"/>
-    <col min="9" max="9" width="13.7109375" customWidth="true"/>
-    <col min="10" max="10" width="6.7109375" customWidth="true"/>
-    <col min="11" max="11" width="11.7109375" customWidth="true"/>
-    <col min="13" max="13" width="7.7109375" customWidth="true"/>
-    <col min="14" max="14" width="11.7109375" customWidth="true"/>
-    <col min="16" max="16" width="13.7109375" customWidth="true"/>
-    <col min="17" max="17" width="17.7109375" customWidth="true"/>
-    <col min="18" max="18" width="12.7109375" customWidth="true"/>
-    <col min="19" max="19" width="6.7109375" customWidth="true"/>
-    <col min="20" max="20" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="6.15625" customWidth="true"/>
+    <col min="4" max="4" width="9.48828125" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.7109375" customWidth="true"/>
     <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="13.37890625" customWidth="true"/>
+    <col min="9" max="9" width="17.7109375" customWidth="true"/>
+    <col min="10" max="10" width="13.7109375" customWidth="true"/>
+    <col min="11" max="11" width="4.7109375" customWidth="true"/>
     <col min="12" max="12" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="7.7109375" customWidth="true"/>
     <col min="15" max="15" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="14.37890625" customWidth="true"/>
+    <col min="18" max="18" width="17.7109375" customWidth="true"/>
+    <col min="19" max="19" width="12.7109375" customWidth="true"/>
+    <col min="20" max="20" width="4.7109375" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
+    <col min="23" max="23" width="3.93359375" customWidth="true"/>
+    <col min="24" max="24" width="12.6640625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="22" max="22" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -533,63 +526,66 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -600,65 +596,65 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>250</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>4.9826449068195009</v>
-      </c>
       <c r="F2">
-        <v>7.9001322104036635</v>
+        <v>4.9765881921048338</v>
       </c>
       <c r="G2">
-        <v>-0.22685820616857416</v>
+        <v>9.1775032916085788</v>
       </c>
       <c r="H2">
-        <v>-0.2073975249232469</v>
+        <v>-0.22605057958873737</v>
       </c>
       <c r="I2">
-        <v>0.59311894177556757</v>
+        <v>-0.20345864393630261</v>
       </c>
       <c r="J2">
-        <v>1.65</v>
+        <v>0.59422294911856732</v>
       </c>
       <c r="K2">
-        <v>2.5037162017088295</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>4.3232609635970078</v>
-      </c>
-      <c r="M2" t="s">
+        <v>2.503578956738028</v>
+      </c>
+      <c r="M2">
+        <v>4.2945330552194125</v>
+      </c>
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2">
-        <v>4.7356539370070294</v>
-      </c>
       <c r="O2">
-        <v>31.65087027615273</v>
+        <v>4.7667584061650476</v>
       </c>
       <c r="P2">
-        <v>5.7096888284919711E-2</v>
+        <v>29.707166694697939</v>
       </c>
       <c r="Q2">
-        <v>-9.3042982720196218E-2</v>
+        <v>5.7951637027478464E-2</v>
       </c>
       <c r="R2">
-        <v>1.1405041982782089</v>
+        <v>-8.5013611188901009E-2</v>
       </c>
       <c r="S2">
-        <v>2.25</v>
+        <v>1.1427510711050559</v>
       </c>
       <c r="T2">
-        <v>2.7323295115112365</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>4.9555216526329442</v>
+        <v>2.71760538339635</v>
       </c>
       <c r="V2">
-        <v>0.5745467581032272</v>
+        <v>4.9292443516885278</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -669,404 +665,351 @@
         <v>18</v>
       </c>
       <c r="C3">
+        <v>20532</v>
+      </c>
+      <c r="D3">
         <v>250</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3">
-        <v>4.9827541319052324</v>
-      </c>
       <c r="F3">
-        <v>7.8740373620503528</v>
+        <v>4.9756980936282016</v>
       </c>
       <c r="G3">
-        <v>-0.22747177973472568</v>
+        <v>9.3453851489789095</v>
       </c>
       <c r="H3">
-        <v>-0.20824049978381717</v>
+        <v>-0.21995478833709303</v>
       </c>
       <c r="I3">
-        <v>0.59228157182295083</v>
+        <v>-0.19734875773931124</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0.60262231802262201</v>
       </c>
       <c r="K3">
-        <v>2.5041788721098985</v>
+        <v>1.65</v>
       </c>
       <c r="L3">
-        <v>4.3239160808207764</v>
-      </c>
-      <c r="M3" t="s">
+        <v>2.5055078612018264</v>
+      </c>
+      <c r="M3">
+        <v>4.2913559820381248</v>
+      </c>
+      <c r="N3" t="s">
         <v>20</v>
       </c>
-      <c r="N3">
-        <v>4.7404864785606913</v>
-      </c>
       <c r="O3">
-        <v>31.350721975264484</v>
+        <v>4.7441370343903682</v>
       </c>
       <c r="P3">
-        <v>5.6693418498374525E-2</v>
+        <v>31.319203131307681</v>
       </c>
       <c r="Q3">
-        <v>-9.1493144296735884E-2</v>
+        <v>6.6914265958757699E-2</v>
       </c>
       <c r="R3">
-        <v>1.1394451350814223</v>
+        <v>-9.3903874771060297E-2</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>1.1665792999957734</v>
       </c>
       <c r="T3">
-        <v>2.729627503259529</v>
+        <v>2.25</v>
       </c>
       <c r="U3">
-        <v>4.9528656752405942</v>
+        <v>2.7100820017831686</v>
       </c>
       <c r="V3">
-        <v>0.57341559073516013</v>
+        <v>4.9858057914476577</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4">
+        <v>20532</v>
+      </c>
+      <c r="D4">
         <v>250</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>4.9997147825811075</v>
+      <c r="E4" t="s">
+        <v>24</v>
       </c>
       <c r="F4">
-        <v>1.0123546844457523</v>
+        <v>4.9743102668471524</v>
       </c>
       <c r="G4">
-        <v>2.1850623651544141</v>
+        <v>9.6124765265976997</v>
       </c>
       <c r="H4">
-        <v>2.1877179967923386</v>
+        <v>-0.33591360224727973</v>
       </c>
       <c r="I4">
-        <v>153.13073432744957</v>
+        <v>-0.31212140633067426</v>
       </c>
       <c r="J4">
-        <v>303.02999999999997</v>
+        <v>0.46140935736715222</v>
       </c>
       <c r="K4">
-        <v>2.4913278861865829</v>
+        <v>1.35</v>
       </c>
       <c r="L4">
-        <v>4.4964457027896536</v>
-      </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4">
-        <v>4.957208825138796</v>
+        <v>2.5048535503349951</v>
+      </c>
+      <c r="M4">
+        <v>4.2852236950365041</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
       </c>
       <c r="O4">
-        <v>12.455041257342652</v>
+        <v>4.7253104329207751</v>
       </c>
       <c r="P4">
-        <v>2.116146697895704</v>
+        <v>32.511602819523866</v>
       </c>
       <c r="Q4">
-        <v>2.1757732740706923</v>
+        <v>-4.1400369814987112E-2</v>
       </c>
       <c r="R4">
-        <v>130.66121667900043</v>
+        <v>-0.20944492255621891</v>
       </c>
       <c r="S4">
-        <v>222.22</v>
+        <v>0.90907482325494815</v>
       </c>
       <c r="T4">
-        <v>2.4563775322756314</v>
+        <v>1.76</v>
       </c>
       <c r="U4">
-        <v>4.2481080206193091</v>
+        <v>2.7144867098447287</v>
       </c>
       <c r="V4">
-        <v>1.1889440487387544</v>
+        <v>5.0133618906442203</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5">
+        <v>20444</v>
+      </c>
+      <c r="D5">
         <v>250</v>
       </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <v>4.6798586414822303</v>
+      <c r="E5" t="s">
+        <v>28</v>
       </c>
       <c r="F5">
-        <v>21.311092513734366</v>
+        <v>4.9734560674494528</v>
       </c>
       <c r="G5">
-        <v>-1.3481989837480159</v>
+        <v>9.7754349569979908</v>
       </c>
       <c r="H5">
-        <v>-1.389217402286778</v>
+        <v>-0.34682998704167944</v>
       </c>
       <c r="I5">
-        <v>4.4853983220576397E-2</v>
+        <v>-0.32280172661921275</v>
       </c>
       <c r="J5">
-        <v>0.67</v>
+        <v>0.44995596436826424</v>
       </c>
       <c r="K5">
-        <v>2.5816969466091404</v>
+        <v>1.35</v>
       </c>
       <c r="L5">
-        <v>3.7150696060018951</v>
-      </c>
-      <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5">
-        <v>4.4875707068022246</v>
+        <v>2.504691751122619</v>
+      </c>
+      <c r="M5">
+        <v>4.2813325868975509</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
       </c>
       <c r="O5">
-        <v>37.001887552688956</v>
+        <v>4.7496601070920921</v>
       </c>
       <c r="P5">
-        <v>-0.64876785580293639</v>
+        <v>30.865071455986872</v>
       </c>
       <c r="Q5">
-        <v>-0.51183675017913821</v>
+        <v>-5.1993857029637276E-2</v>
       </c>
       <c r="R5">
-        <v>0.22450816705765561</v>
+        <v>-0.20505853243373351</v>
       </c>
       <c r="S5">
-        <v>0.44</v>
+        <v>0.88716856069298433</v>
       </c>
       <c r="T5">
-        <v>2.7441176564680601</v>
+        <v>1.76</v>
       </c>
       <c r="U5">
-        <v>4.0971384291796884</v>
+        <v>2.7183490275012758</v>
       </c>
       <c r="V5">
-        <v>0.23414038748356941</v>
+        <v>4.9627952919200915</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>500</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6">
-        <v>4.7026976035184864</v>
+        <v>20532</v>
+      </c>
+      <c r="D6">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
       </c>
       <c r="F6">
-        <v>19.255097091802149</v>
+        <v>4.6519035218226765</v>
       </c>
       <c r="G6">
-        <v>-1.3362678808654391</v>
+        <v>23.610134507308679</v>
       </c>
       <c r="H6">
-        <v>-1.3941377130566481</v>
+        <v>-1.3117277829692866</v>
       </c>
       <c r="I6">
-        <v>4.6103311309136655E-2</v>
+        <v>-1.350080204977842</v>
       </c>
       <c r="J6">
-        <v>0.62</v>
+        <v>4.8783417015415241E-2</v>
       </c>
       <c r="K6">
-        <v>2.6016446203947199</v>
+        <v>0.71</v>
       </c>
       <c r="L6">
-        <v>3.8350165554762237</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6">
-        <v>4.4612663544296156</v>
+        <v>2.5925087875061656</v>
+      </c>
+      <c r="M6">
+        <v>3.663436355060171</v>
+      </c>
+      <c r="N6" t="s">
+        <v>33</v>
       </c>
       <c r="O6">
-        <v>38.786048126058219</v>
+        <v>4.4670217174170981</v>
       </c>
       <c r="P6">
-        <v>-0.63296529236637555</v>
+        <v>38.279552720015474</v>
       </c>
       <c r="Q6">
-        <v>-0.5012775858011308</v>
+        <v>-0.57433331148383981</v>
       </c>
       <c r="R6">
-        <v>0.23282773198201309</v>
+        <v>-0.40770100046678204</v>
       </c>
       <c r="S6">
-        <v>0.4</v>
+        <v>0.2664812694242375</v>
       </c>
       <c r="T6">
-        <v>2.76557150664777</v>
+        <v>0.49</v>
       </c>
       <c r="U6">
-        <v>4.0668101682719353</v>
+        <v>2.7344474715628291</v>
       </c>
       <c r="V6">
-        <v>0.23539846667524203</v>
+        <v>4.0480756280027492</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C7">
-        <v>500</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E7">
-        <v>4.7906418405145521</v>
-      </c>
-      <c r="F7">
-        <v>7.8095861425232034</v>
-      </c>
-      <c r="G7">
-        <v>2.0677957682929509</v>
-      </c>
-      <c r="H7">
-        <v>2.0736812204762769</v>
-      </c>
-      <c r="I7">
-        <v>116.89495504965939</v>
-      </c>
-      <c r="J7">
-        <v>500</v>
-      </c>
-      <c r="K7">
-        <v>2.4955351463113833</v>
-      </c>
-      <c r="L7">
-        <v>4.1235868656811236</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="C7" s="0">
+        <v>20242</v>
+      </c>
+      <c r="D7" s="0">
+        <v>125</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="N7">
-        <v>4.7126536062264037</v>
-      </c>
-      <c r="O7">
-        <v>18.377104569427054</v>
-      </c>
-      <c r="P7">
-        <v>2.0355298942327686</v>
-      </c>
-      <c r="Q7">
-        <v>2.0220858840864073</v>
-      </c>
-      <c r="R7">
-        <v>108.52502491934652</v>
-      </c>
-      <c r="S7">
-        <v>500</v>
-      </c>
-      <c r="T7">
-        <v>2.4589208462812953</v>
-      </c>
-      <c r="U7">
-        <v>4.2481821928316998</v>
-      </c>
-      <c r="V7">
-        <v>1.099828617014579</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
+      <c r="F7" s="0">
+        <v>4.656250519195309</v>
+      </c>
+      <c r="G7" s="0">
+        <v>23.351665561199709</v>
+      </c>
+      <c r="H7" s="0">
+        <v>-1.3656359134406633</v>
+      </c>
+      <c r="I7" s="0">
+        <v>-1.4063430082057606</v>
+      </c>
+      <c r="J7" s="0">
+        <v>0.043088768962510196</v>
+      </c>
+      <c r="K7" s="0">
+        <v>0.70999999999999996</v>
+      </c>
+      <c r="L7" s="0">
+        <v>2.5739275762624128</v>
+      </c>
+      <c r="M7" s="0">
+        <v>3.6663453879814232</v>
+      </c>
+      <c r="N7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="0">
-        <v>500</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="0">
-        <v>4.7906418405145521</v>
-      </c>
-      <c r="F8" s="0">
-        <v>7.8095861425232034</v>
-      </c>
-      <c r="G8" s="0">
-        <v>2.0677957682929509</v>
-      </c>
-      <c r="H8" s="0">
-        <v>2.0736812204762769</v>
-      </c>
-      <c r="I8" s="0">
-        <v>116.89495504965939</v>
-      </c>
-      <c r="J8" s="0">
-        <v>500</v>
-      </c>
-      <c r="K8" s="0">
-        <v>2.4955351463113833</v>
-      </c>
-      <c r="L8" s="0">
-        <v>4.1235868656811236</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="0">
-        <v>4.7126536062264037</v>
-      </c>
-      <c r="O8" s="0">
-        <v>18.377104569427054</v>
-      </c>
-      <c r="P8" s="0">
-        <v>2.0355298942327686</v>
-      </c>
-      <c r="Q8" s="0">
-        <v>2.0220858840864073</v>
-      </c>
-      <c r="R8" s="0">
-        <v>108.52502491934652</v>
-      </c>
-      <c r="S8" s="0">
-        <v>500</v>
-      </c>
-      <c r="T8" s="0">
-        <v>2.4589208462812953</v>
-      </c>
-      <c r="U8" s="0">
-        <v>4.2481821928316998</v>
-      </c>
-      <c r="V8" s="0">
-        <v>1.099828617014579</v>
+      <c r="O7" s="0">
+        <v>4.4800139655585349</v>
+      </c>
+      <c r="P7" s="0">
+        <v>37.525118660511062</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>-0.67969225932921751</v>
+      </c>
+      <c r="R7" s="0">
+        <v>-0.53173571411195641</v>
+      </c>
+      <c r="S7" s="0">
+        <v>0.209077712882734</v>
+      </c>
+      <c r="T7" s="0">
+        <v>0.48999999999999999</v>
+      </c>
+      <c r="U7" s="0">
+        <v>2.7511413305687156</v>
+      </c>
+      <c r="V7" s="0">
+        <v>4.0248403394561594</v>
+      </c>
+      <c r="W7" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major update, added new class
* user can add upto 4 grids in settings (32 or 64)
</commit_message>
<xml_diff>
--- a/MainReport.xlsx
+++ b/MainReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprad\Documents\MATLAB\Project_UK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F45AAE-07D6-42A2-BACB-26B28E7CD6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D8DA57-F02C-4CCA-8DD2-F0829F1DC5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView minimized="true" xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Filename</t>
   </si>
@@ -134,6 +134,42 @@
   </si>
   <si>
     <t>grid2:28</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>MDF</t>
+  </si>
+  <si>
+    <t>Grid1: 32</t>
+  </si>
+  <si>
+    <t>Grid2: 32</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Grid1: 32</t>
+  </si>
+  <si>
+    <t>Grid2: 32</t>
+  </si>
+  <si>
+    <t>L120.csv</t>
+  </si>
+  <si>
+    <t>MDF</t>
+  </si>
+  <si>
+    <t>Grid1: 32</t>
+  </si>
+  <si>
+    <t>Grid2: 32</t>
   </si>
 </sst>
 </file>
@@ -484,9 +520,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -496,14 +532,14 @@
     <col min="2" max="2" width="7.37890625" customWidth="true"/>
     <col min="3" max="3" width="6.15625" customWidth="true"/>
     <col min="4" max="4" width="9.48828125" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="7.7109375" customWidth="true"/>
+    <col min="5" max="5" width="8.48828125" customWidth="true"/>
     <col min="6" max="6" width="11.7109375" customWidth="true"/>
     <col min="8" max="8" width="13.37890625" customWidth="true"/>
     <col min="9" max="9" width="17.7109375" customWidth="true"/>
     <col min="10" max="10" width="13.7109375" customWidth="true"/>
     <col min="11" max="11" width="4.7109375" customWidth="true"/>
     <col min="12" max="12" width="11.7109375" customWidth="true"/>
-    <col min="14" max="14" width="7.7109375" customWidth="true"/>
+    <col min="14" max="14" width="8.48828125" customWidth="true"/>
     <col min="15" max="15" width="11.7109375" customWidth="true"/>
     <col min="17" max="17" width="14.37890625" customWidth="true"/>
     <col min="18" max="18" width="17.7109375" customWidth="true"/>
@@ -942,73 +978,286 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="s">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>20242</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>125</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>4.656250519195309</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>23.351665561199709</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>-1.3656359134406633</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>-1.4063430082057606</v>
       </c>
-      <c r="J7" s="0">
-        <v>0.043088768962510196</v>
-      </c>
-      <c r="K7" s="0">
-        <v>0.70999999999999996</v>
-      </c>
-      <c r="L7" s="0">
+      <c r="J7">
+        <v>4.3088768962510196E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.71</v>
+      </c>
+      <c r="L7">
         <v>2.5739275762624128</v>
       </c>
-      <c r="M7" s="0">
+      <c r="M7">
         <v>3.6663453879814232</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <v>4.4800139655585349</v>
       </c>
-      <c r="P7" s="0">
+      <c r="P7">
         <v>37.525118660511062</v>
       </c>
-      <c r="Q7" s="0">
+      <c r="Q7">
         <v>-0.67969225932921751</v>
       </c>
-      <c r="R7" s="0">
+      <c r="R7">
         <v>-0.53173571411195641</v>
       </c>
-      <c r="S7" s="0">
+      <c r="S7">
         <v>0.209077712882734</v>
       </c>
-      <c r="T7" s="0">
-        <v>0.48999999999999999</v>
-      </c>
-      <c r="U7" s="0">
+      <c r="T7">
+        <v>0.49</v>
+      </c>
+      <c r="U7">
         <v>2.7511413305687156</v>
       </c>
-      <c r="V7" s="0">
+      <c r="V7">
         <v>4.0248403394561594</v>
       </c>
-      <c r="W7" s="0">
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>20282</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>4.9997147825811075</v>
+      </c>
+      <c r="G8">
+        <v>1.0123546844457523</v>
+      </c>
+      <c r="H8">
+        <v>2.1850623651544141</v>
+      </c>
+      <c r="I8">
+        <v>2.1877179967923386</v>
+      </c>
+      <c r="J8">
+        <v>153.13073432744957</v>
+      </c>
+      <c r="K8">
+        <v>500</v>
+      </c>
+      <c r="L8">
+        <v>2.4913278861865829</v>
+      </c>
+      <c r="M8">
+        <v>4.4964457027896536</v>
+      </c>
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8">
+        <v>4.957208825138796</v>
+      </c>
+      <c r="P8">
+        <v>12.455041257342652</v>
+      </c>
+      <c r="Q8">
+        <v>2.116146697895704</v>
+      </c>
+      <c r="R8">
+        <v>2.1757732740706923</v>
+      </c>
+      <c r="S8">
+        <v>130.66121667900043</v>
+      </c>
+      <c r="T8">
+        <v>500</v>
+      </c>
+      <c r="U8">
+        <v>2.4563775322756314</v>
+      </c>
+      <c r="V8">
+        <v>4.2481080206193091</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>20282</v>
+      </c>
+      <c r="D9">
+        <v>250</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9">
+        <v>4.9827541319052324</v>
+      </c>
+      <c r="G9">
+        <v>7.8740373620503528</v>
+      </c>
+      <c r="H9">
+        <v>-0.22747177973472568</v>
+      </c>
+      <c r="I9">
+        <v>-0.20824049978381717</v>
+      </c>
+      <c r="J9">
+        <v>0.59228157182295083</v>
+      </c>
+      <c r="K9">
+        <v>1.65</v>
+      </c>
+      <c r="L9">
+        <v>2.5041788721098985</v>
+      </c>
+      <c r="M9">
+        <v>4.3239160808207764</v>
+      </c>
+      <c r="N9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9">
+        <v>4.7404864785606913</v>
+      </c>
+      <c r="P9">
+        <v>31.350721975264484</v>
+      </c>
+      <c r="Q9">
+        <v>5.6693418498374525E-2</v>
+      </c>
+      <c r="R9">
+        <v>-9.1493144296735884E-2</v>
+      </c>
+      <c r="S9">
+        <v>1.1394451350814223</v>
+      </c>
+      <c r="T9">
+        <v>2.25</v>
+      </c>
+      <c r="U9">
+        <v>2.729627503259529</v>
+      </c>
+      <c r="V9">
+        <v>4.9528656752405942</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="0">
+        <v>20282</v>
+      </c>
+      <c r="D10" s="0">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="0">
+        <v>4.9899433448642005</v>
+      </c>
+      <c r="G10" s="0">
+        <v>5.9604783568598751</v>
+      </c>
+      <c r="H10" s="0">
+        <v>2.0400266820151334</v>
+      </c>
+      <c r="I10" s="0">
+        <v>2.0344533587457043</v>
+      </c>
+      <c r="J10" s="0">
+        <v>109.65455632127134</v>
+      </c>
+      <c r="K10" s="0">
+        <v>500</v>
+      </c>
+      <c r="L10" s="0">
+        <v>2.5060892817466955</v>
+      </c>
+      <c r="M10" s="0">
+        <v>4.4042009296413376</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="0">
+        <v>4.9517624780973328</v>
+      </c>
+      <c r="P10" s="0">
+        <v>13.285536622456886</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>2.0679762691188244</v>
+      </c>
+      <c r="R10" s="0">
+        <v>2.1299249175009325</v>
+      </c>
+      <c r="S10" s="0">
+        <v>116.94354885435517</v>
+      </c>
+      <c r="T10" s="0">
+        <v>500</v>
+      </c>
+      <c r="U10" s="0">
+        <v>2.4427652631336318</v>
+      </c>
+      <c r="V10" s="0">
+        <v>4.2369687702681196</v>
+      </c>
+      <c r="W10" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>